<commit_message>
working at UI (Designer).
</commit_message>
<xml_diff>
--- a/UIDesign/assets/texts/texts.xlsx
+++ b/UIDesign/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1360" uniqueCount="75">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -156,6 +156,90 @@
   </si>
   <si>
     <t xml:space="preserve">Start</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Left</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pippo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TextAreaRes1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ButtonText1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pippo </t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;*&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Counter&lt;*&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Counter: &lt;*&gt;&lt;*&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Count</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Counter: &lt;**&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Counter: &lt;c&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Counter: &lt;counter&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Counter: &lt;counter&gt;&lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Counter: &lt;counter_&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Counter: &lt;counter_value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0,9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0123456789</t>
   </si>
 </sst>
 </file>
@@ -1381,7 +1465,9 @@
       <c r="F4" t="s">
         <v>17</v>
       </c>
-      <c r="G4"/>
+      <c r="G4" t="s">
+        <v>74</v>
+      </c>
       <c r="H4"/>
       <c r="I4"/>
       <c r="K4" s="4" t="s">
@@ -1614,6 +1700,58 @@
         <v>46</v>
       </c>
     </row>
+    <row r="5">
+      <c r="B5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
modified the UI for the visual shortcuts.
</commit_message>
<xml_diff>
--- a/UIDesign/assets/texts/texts.xlsx
+++ b/UIDesign/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1516" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1537" uniqueCount="78">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -1709,57 +1709,9 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5">
-      <c r="B5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D5" t="s">
-        <v>49</v>
-      </c>
-      <c r="E5" t="s">
-        <v>43</v>
-      </c>
-      <c r="F5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="B6" t="s">
-        <v>48</v>
-      </c>
-      <c r="C6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D6" t="s">
-        <v>42</v>
-      </c>
-      <c r="E6" t="s">
-        <v>43</v>
-      </c>
-      <c r="F6" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="B7" t="s">
-        <v>63</v>
-      </c>
-      <c r="C7" t="s">
-        <v>37</v>
-      </c>
-      <c r="D7" t="s">
-        <v>49</v>
-      </c>
-      <c r="E7" t="s">
-        <v>43</v>
-      </c>
-      <c r="F7" t="s">
-        <v>71</v>
-      </c>
-    </row>
+    <row r="5"/>
+    <row r="6"/>
+    <row r="7"/>
     <row r="8"/>
   </sheetData>
   <mergeCells count="1">

</xml_diff>